<commit_message>
Updating geography for point locations (closes #38) and ward code gazeteers (#29)
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -11,11 +11,10 @@
     <s:sheet name="Classification" sheetId="2" r:id="rId2"/>
     <s:sheet name="Documents" sheetId="3" r:id="rId3"/>
     <s:sheet name="Event" sheetId="4" r:id="rId4"/>
-    <s:sheet name="Gazeteer" sheetId="5" r:id="rId5"/>
-    <s:sheet name="GrantProgramme" sheetId="6" r:id="rId6"/>
-    <s:sheet name="Location" sheetId="7" r:id="rId7"/>
-    <s:sheet name="Organization" sheetId="8" r:id="rId8"/>
-    <s:sheet name="Transaction" sheetId="9" r:id="rId9"/>
+    <s:sheet name="GrantProgramme" sheetId="5" r:id="rId5"/>
+    <s:sheet name="Location" sheetId="6" r:id="rId6"/>
+    <s:sheet name="Organization" sheetId="7" r:id="rId7"/>
+    <s:sheet name="Transaction" sheetId="8" r:id="rId8"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -100,24 +99,6 @@
     <t>duration</t>
   </si>
   <si>
-    <t>Activity/id:gazeteerEntry</t>
-  </si>
-  <si>
-    <t>Activity/recipientOrganization[]/id:gazeteerEntry</t>
-  </si>
-  <si>
-    <t>Activity/recipientOrganization[]/location[]/id:gazeteerEntry</t>
-  </si>
-  <si>
-    <t>Activity/beneficiaryLocation[]/id:gazeteerEntry</t>
-  </si>
-  <si>
-    <t>Activity/fundingOrganization[]/id:gazeteerEntry</t>
-  </si>
-  <si>
-    <t>Activity/fundingOrganization[]/location[]/id:gazeteerEntry</t>
-  </si>
-  <si>
     <t>Activity/id:grantProgramme</t>
   </si>
   <si>
@@ -139,7 +120,16 @@
     <t>countryCode</t>
   </si>
   <si>
-    <t>point</t>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>geoCode</t>
+  </si>
+  <si>
+    <t>geoCodeType</t>
   </si>
   <si>
     <t>Activity/id:recipientOrganization</t>
@@ -738,65 +728,6 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -810,7 +741,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -833,12 +764,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,38 +777,47 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -886,7 +826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -904,55 +844,55 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" t="s">
-        <v>51</v>
       </c>
       <c r="Q1" t="s">
         <v>2</v>
       </c>
       <c r="R1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="S1" t="s">
         <v>3</v>
@@ -966,7 +906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -984,37 +924,37 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Re-ordering fields. Adding required fields. Updating guidance. Closes #40, #39
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -33,21 +33,24 @@
     <t>description</t>
   </si>
   <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>amountAppliedFor:number</t>
+  </si>
+  <si>
+    <t>amountAwarded:number</t>
+  </si>
+  <si>
+    <t>amountDisbursed:number</t>
+  </si>
+  <si>
+    <t>awardDate</t>
+  </si>
+  <si>
     <t>url</t>
   </si>
   <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>amountAppliedFor:number</t>
-  </si>
-  <si>
-    <t>amountAwarded:number</t>
-  </si>
-  <si>
-    <t>amountDisbursed:number</t>
-  </si>
-  <si>
     <t>fromOpenCall</t>
   </si>
   <si>
@@ -84,9 +87,6 @@
     <t>Activity/id:plannedDates</t>
   </si>
   <si>
-    <t>Activity/id:awardDate</t>
-  </si>
-  <si>
     <t>Activity/id:actualDates</t>
   </si>
   <si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Activity/id:fundingOrganization</t>
+  </si>
+  <si>
+    <t>department</t>
   </si>
   <si>
     <t>contactName</t>
@@ -531,7 +534,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +542,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,6 +578,9 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -597,19 +603,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -618,10 +624,10 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -644,10 +650,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -656,16 +662,16 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -678,7 +684,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,36 +692,33 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -738,13 +741,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -753,10 +756,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +782,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -818,7 +821,7 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +834,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,9 +842,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
@@ -889,16 +892,19 @@
         <v>48</v>
       </c>
       <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
-        <v>49</v>
-      </c>
       <c r="S1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="T1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="U1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -921,43 +927,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing ocid entry from spreadsheet template. Fixes #46
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>dataSource</t>
-  </si>
-  <si>
-    <t>ocid</t>
   </si>
   <si>
     <t>Activity/id:fundingType</t>
@@ -593,7 +590,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,7 +598,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -615,18 +612,15 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -636,6 +630,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -650,25 +685,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -679,12 +714,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -692,32 +727,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -726,193 +752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -927,7 +767,146 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins right="0.75" footer="0.5" top="1" bottom="1" header="0.5" left="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
@@ -936,33 +915,30 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
       </c>
       <c r="H1" t="s">
         <v>55</v>
       </c>
       <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
       </c>
       <c r="K1" t="s">
         <v>57</v>
       </c>
       <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Document grant package schema
This should also address #81 and #82
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -540,48 +540,48 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c t="s" r="I1">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c t="s" r="K1">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c t="s" r="M1">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -599,33 +599,33 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -643,30 +643,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -684,33 +684,33 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -728,27 +728,27 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -766,48 +766,48 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c t="s" r="I1">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c t="s" r="K1">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c t="s" r="M1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -825,69 +825,69 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c t="s" r="I1">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c t="s" r="K1">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c t="s" r="M1">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c t="s" r="N1">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c t="s" r="O1">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c t="s" r="P1">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c t="s" r="Q1">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
+      <c t="s" r="R1">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c t="s" r="S1">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c t="s" r="T1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
 
@@ -905,44 +905,44 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c t="s" r="I1">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>56</v>
       </c>
-      <c r="K1" t="s">
+      <c t="s" r="K1">
         <v>57</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" footer="0.5" left="0.75" header="0.5"/>
+  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improves documentation to make the two schemas more distinct
Now we have two schemas to talk about it seems easier to talk about
360Giving Grant Schema, and the the 360Giving Package Schema
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -1,10 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:workbookPr/>
   <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
     <s:sheet name="Transaction" sheetId="8" r:id="rId8"/>
   </s:sheets>
   <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
@@ -205,10 +204,10 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -527,10 +526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -540,56 +539,56 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="K1">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="L1">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="M1">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -599,41 +598,41 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -643,38 +642,38 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -684,41 +683,41 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -728,35 +727,35 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -766,56 +765,56 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="K1">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="L1">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="M1">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -825,77 +824,77 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c t="s" r="K1">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="L1">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="M1">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="N1">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="O1">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c t="s" r="P1">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="Q1">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="R1">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="S1">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="T1">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr>
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+  </s:sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -905,44 +904,44 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c t="s" r="K1">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c t="s" r="L1">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" left="0.75" bottom="1" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix flattentool egg name to work with older versions of pip
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -1,9 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <s:bookViews>
-    <s:workbookView activeTab="0"/>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
     <s:sheet name="Transaction" sheetId="8" r:id="rId8"/>
   </s:sheets>
   <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
@@ -204,10 +205,10 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -526,10 +527,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -580,15 +581,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -624,15 +625,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -665,15 +666,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -709,15 +710,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -747,15 +748,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -806,15 +807,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -886,15 +887,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -942,6 +943,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[#89] country in rollUp should be addressCountry
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -527,7 +527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -581,12 +581,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -625,12 +625,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -666,12 +666,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -710,12 +710,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -748,12 +748,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -807,12 +807,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -887,12 +887,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -943,6 +943,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" bottom="1" footer="0.5" top="1" right="0.75" left="0.75"/>
+  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[#89] Add addressRegion (County) to rollUp
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -527,7 +527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -581,12 +581,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -625,12 +625,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -666,12 +666,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -710,12 +710,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -748,12 +748,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -807,12 +807,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -887,12 +887,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -943,6 +943,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" bottom="1" left="0.75" footer="0.5" header="0.5" right="0.75"/>
+  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update flatten-tool and its dependencies
</commit_message>
<xml_diff>
--- a/schema/multi-table/360-giving-schema-fields.xlsx
+++ b/schema/multi-table/360-giving-schema-fields.xlsx
@@ -1,10 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:workbookPr/>
   <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
     <s:sheet name="Transaction" sheetId="8" r:id="rId8"/>
   </s:sheets>
   <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
@@ -205,16 +204,16 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -236,7 +235,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -527,9 +526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -581,14 +581,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -625,14 +626,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -666,14 +668,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -710,14 +713,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -748,14 +752,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -807,14 +812,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:T1"/>
   <sheetViews>
@@ -887,14 +893,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -943,6 +950,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>